<commit_message>
replaced package xlsx with openxlsx which has no java dependency
</commit_message>
<xml_diff>
--- a/inst/extdata/data3/output_files_96w/output/trt_P11.xlsx
+++ b/inst/extdata/data3/output_files_96w/output/trt_P11.xlsx
@@ -1,74 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Gnumber" r:id="rId3" sheetId="1"/>
-    <sheet name="Concentration" r:id="rId4" sheetId="2"/>
+    <sheet name="Gnumber" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Concentration" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="15">
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>G00004</t>
-  </si>
-  <si>
-    <t>G00005</t>
-  </si>
-  <si>
-    <t>G00006</t>
-  </si>
-  <si>
-    <t>vehicle</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>3.162277660168</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0.3162277660168</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.03162277660168</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>0.003162277660168</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>0</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">G00004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G00005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G00006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.162277660168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3162277660168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03162277660168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.003162277660168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11.0"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,7 +79,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -97,16 +97,297 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -175,7 +456,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -210,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -218,34 +499,34 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
         <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -253,34 +534,34 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
         <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -288,34 +569,34 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -323,48 +604,49 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -612,6 +894,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>